<commit_message>
duplicate container data merged
</commit_message>
<xml_diff>
--- a/reports/_ABL_SUMMIT ALLIANCE PORT LIMITED_container_report_2018-12-03_35_.xlsx
+++ b/reports/_ABL_SUMMIT ALLIANCE PORT LIMITED_container_report_2018-12-03_35_.xlsx
@@ -1555,7 +1555,7 @@
           <t>CEPZ</t>
         </is>
       </c>
-      <c r="M6" s="0" t="d">
+      <c r="M6" s="4" t="d">
         <v>2018-10-01T09:53:38.14</v>
       </c>
       <c r="N6" s="0" t="inlineStr">
@@ -1577,7 +1577,7 @@
       </c>
       <c r="S6" s="0"/>
       <c r="T6" s="0"/>
-      <c r="U6" s="0"/>
+      <c r="U6" s="4"/>
       <c r="V6" s="0"/>
       <c r="W6" s="0"/>
       <c r="X6" s="0"/>

</xml_diff>